<commit_message>
Plot E/I clusters. Increase strictness of applyQualityMetrics
edit to never move a unit labelled as "mua" by kilosort to "good"
</commit_message>
<xml_diff>
--- a/src/kilosort_config_files/SILICON PROBE MAP F.xlsx
+++ b/src/kilosort_config_files/SILICON PROBE MAP F.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Dropbox\alab\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Dropbox\alab\Code\spikesort\spikesort-hp\src\kilosort_config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="19">
   <si>
     <t>E</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>ypos</t>
+  </si>
+  <si>
+    <t>IntanChannel</t>
+  </si>
+  <si>
+    <t>MolexChannel</t>
+  </si>
+  <si>
+    <t>ShankLetter</t>
+  </si>
+  <si>
+    <t>ShankPosition</t>
   </si>
 </sst>
 </file>
@@ -178,10 +190,10 @@
     <sortCondition ref="C1:C65"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Intan channel" dataDxfId="5"/>
-    <tableColumn id="2" name="Molex channel" dataDxfId="4"/>
-    <tableColumn id="3" name="Shank Letter" dataDxfId="3"/>
-    <tableColumn id="5" name="Shank Position" dataDxfId="2"/>
+    <tableColumn id="1" name="IntanChannel" dataDxfId="5"/>
+    <tableColumn id="2" name="MolexChannel" dataDxfId="4"/>
+    <tableColumn id="3" name="ShankLetter" dataDxfId="3"/>
+    <tableColumn id="5" name="ShankPosition" dataDxfId="2"/>
     <tableColumn id="4" name="xpos" dataDxfId="1"/>
     <tableColumn id="6" name="ypos" dataDxfId="0"/>
   </tableColumns>
@@ -455,7 +467,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="D12:E22"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,16 +479,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>

</xml_diff>